<commit_message>
updated code for the failures
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataCMS/AI_Timesheets.xlsx
+++ b/src/test/resources/testdataCMS/AI_Timesheets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
   <si>
     <t>Employee Name</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>11/24/2024</t>
+  </si>
+  <si>
+    <t>Ray Beer</t>
   </si>
 </sst>
 </file>
@@ -315,7 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -352,6 +355,30 @@
     </xf>
     <xf numFmtId="46" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
@@ -1083,8 +1110,8 @@
       <c r="C6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="141" t="s">
-        <v>62</v>
+      <c r="D6" s="149" t="s">
+        <v>70</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>1</v>
@@ -1146,8 +1173,8 @@
       </c>
     </row>
     <row r="10" spans="2:16">
-      <c r="C10" s="142" t="s">
-        <v>63</v>
+      <c r="C10" s="150" t="s">
+        <v>29</v>
       </c>
       <c r="D10" s="9">
         <v>0.20833333333333334</v>
@@ -1166,8 +1193,8 @@
       </c>
     </row>
     <row r="11" spans="2:16">
-      <c r="C11" s="143" t="s">
-        <v>64</v>
+      <c r="C11" s="151" t="s">
+        <v>30</v>
       </c>
       <c r="D11" s="9">
         <v>0.33333333333333331</v>
@@ -1186,8 +1213,8 @@
       </c>
     </row>
     <row r="12" spans="2:16">
-      <c r="C12" s="144" t="s">
-        <v>65</v>
+      <c r="C12" s="152" t="s">
+        <v>31</v>
       </c>
       <c r="D12" s="9">
         <v>0.29166666666666669</v>
@@ -1206,8 +1233,8 @@
       </c>
     </row>
     <row r="13" spans="2:16">
-      <c r="C13" s="145" t="s">
-        <v>66</v>
+      <c r="C13" s="153" t="s">
+        <v>32</v>
       </c>
       <c r="D13" s="9">
         <v>0.33333333333333331</v>
@@ -1226,8 +1253,8 @@
       </c>
     </row>
     <row r="14" spans="2:16">
-      <c r="C14" s="146" t="s">
-        <v>67</v>
+      <c r="C14" s="154" t="s">
+        <v>33</v>
       </c>
       <c r="D14" s="9">
         <v>0.33333333333333331</v>
@@ -1246,8 +1273,8 @@
       </c>
     </row>
     <row r="15" spans="2:16">
-      <c r="C15" s="147" t="s">
-        <v>68</v>
+      <c r="C15" s="155" t="s">
+        <v>34</v>
       </c>
       <c r="D15" s="9">
         <v>0.33333333333333331</v>
@@ -1266,8 +1293,8 @@
       </c>
     </row>
     <row r="16" spans="2:16">
-      <c r="C16" s="148" t="s">
-        <v>69</v>
+      <c r="C16" s="156" t="s">
+        <v>35</v>
       </c>
       <c r="D16" s="9">
         <v>0.33333333333333331</v>

</xml_diff>